<commit_message>
Updated existing and added new legacy excel sheet test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/sheets/csam-plc-lsac-alarms.xlsx
+++ b/src/test/resources/sheets/csam-plc-lsac-alarms.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="527">
   <si>
     <t>CSAM </t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>DERANGEMENT_INSTALLATION</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
   <si>
     <t>MEY</t>
@@ -3515,8 +3518,8 @@
   </sheetPr>
   <dimension ref="A1:CL56"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="AO1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="AU43" activeCellId="0" pane="topLeft" sqref="AU43"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="A14" activeCellId="1" pane="topLeft" sqref="R8 A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4210,7 +4213,7 @@
       <c r="BK7" s="51"/>
       <c r="BL7" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="8" s="88">
       <c r="A8" s="67"/>
       <c r="B8" s="68" t="n">
         <v>1501016</v>
@@ -4246,9 +4249,11 @@
       <c r="M8" s="72" t="n">
         <v>2</v>
       </c>
-      <c r="N8" s="73"/>
+      <c r="N8" s="73" t="s">
+        <v>84</v>
+      </c>
       <c r="O8" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P8" s="75" t="n">
         <v>27</v>
@@ -4256,18 +4261,20 @@
       <c r="Q8" s="75" t="n">
         <v>2008</v>
       </c>
-      <c r="R8" s="75"/>
+      <c r="R8" s="75" t="s">
+        <v>84</v>
+      </c>
       <c r="S8" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T8" s="76" t="n">
         <v>3</v>
       </c>
       <c r="U8" s="77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V8" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W8" s="78"/>
       <c r="X8" s="77"/>
@@ -4280,16 +4287,16 @@
         <v>7</v>
       </c>
       <c r="AC8" s="80" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="AD8" s="81" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE8" s="80" t="n">
         <v>4</v>
       </c>
       <c r="AF8" s="81" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AG8" s="82"/>
       <c r="AH8" s="82"/>
@@ -4315,10 +4322,10 @@
       <c r="BB8" s="86"/>
       <c r="BC8" s="86"/>
       <c r="BD8" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BE8" s="72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BH8" s="51"/>
       <c r="BI8" s="51"/>
@@ -4326,7 +4333,7 @@
       <c r="BK8" s="51"/>
       <c r="BL8" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="9" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="9" s="88">
       <c r="A9" s="67"/>
       <c r="B9" s="68" t="n">
         <v>1501016</v>
@@ -4335,7 +4342,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="69" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E9" s="69" t="s">
         <v>80</v>
@@ -4354,7 +4361,7 @@
       </c>
       <c r="J9" s="70"/>
       <c r="K9" s="69" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L9" s="71" t="n">
         <v>0</v>
@@ -4364,7 +4371,7 @@
       </c>
       <c r="N9" s="73"/>
       <c r="O9" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P9" s="75" t="n">
         <v>27</v>
@@ -4374,16 +4381,16 @@
       </c>
       <c r="R9" s="75"/>
       <c r="S9" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T9" s="76" t="n">
         <v>3</v>
       </c>
       <c r="U9" s="77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V9" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W9" s="78"/>
       <c r="X9" s="77"/>
@@ -4399,13 +4406,13 @@
         <v>6</v>
       </c>
       <c r="AD9" s="81" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE9" s="80" t="n">
         <v>4</v>
       </c>
       <c r="AF9" s="81" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AG9" s="82"/>
       <c r="AH9" s="82"/>
@@ -4431,10 +4438,10 @@
       <c r="BB9" s="86"/>
       <c r="BC9" s="86"/>
       <c r="BD9" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BE9" s="72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BH9" s="51"/>
       <c r="BI9" s="51"/>
@@ -4442,7 +4449,7 @@
       <c r="BK9" s="51"/>
       <c r="BL9" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="10" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="10" s="88">
       <c r="A10" s="67"/>
       <c r="B10" s="68" t="n">
         <v>1501016</v>
@@ -4451,7 +4458,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="69" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E10" s="69" t="s">
         <v>80</v>
@@ -4470,7 +4477,7 @@
       </c>
       <c r="J10" s="70"/>
       <c r="K10" s="69" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L10" s="71" t="n">
         <v>0</v>
@@ -4480,7 +4487,7 @@
       </c>
       <c r="N10" s="73"/>
       <c r="O10" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P10" s="75" t="n">
         <v>27</v>
@@ -4490,16 +4497,16 @@
       </c>
       <c r="R10" s="75"/>
       <c r="S10" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T10" s="76" t="n">
         <v>401</v>
       </c>
       <c r="U10" s="77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V10" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W10" s="78"/>
       <c r="X10" s="77"/>
@@ -4515,13 +4522,13 @@
         <v>10</v>
       </c>
       <c r="AD10" s="81" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE10" s="80" t="n">
         <v>4</v>
       </c>
       <c r="AF10" s="81" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AG10" s="82"/>
       <c r="AH10" s="82"/>
@@ -4547,10 +4554,10 @@
       <c r="BB10" s="86"/>
       <c r="BC10" s="86"/>
       <c r="BD10" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BE10" s="72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BH10" s="51"/>
       <c r="BI10" s="51"/>
@@ -4558,7 +4565,7 @@
       <c r="BK10" s="51"/>
       <c r="BL10" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="11" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="11" s="88">
       <c r="A11" s="67"/>
       <c r="B11" s="68" t="n">
         <v>1501016</v>
@@ -4567,7 +4574,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="69" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E11" s="69" t="s">
         <v>80</v>
@@ -4586,7 +4593,7 @@
       </c>
       <c r="J11" s="70"/>
       <c r="K11" s="69" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L11" s="71" t="n">
         <v>0</v>
@@ -4596,7 +4603,7 @@
       </c>
       <c r="N11" s="73"/>
       <c r="O11" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P11" s="75" t="n">
         <v>27</v>
@@ -4606,16 +4613,16 @@
       </c>
       <c r="R11" s="75"/>
       <c r="S11" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T11" s="76" t="n">
         <v>1</v>
       </c>
       <c r="U11" s="77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V11" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W11" s="78"/>
       <c r="X11" s="77"/>
@@ -4631,13 +4638,13 @@
         <v>9</v>
       </c>
       <c r="AD11" s="81" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE11" s="80" t="n">
         <v>4</v>
       </c>
       <c r="AF11" s="81" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AG11" s="82"/>
       <c r="AH11" s="82"/>
@@ -4663,10 +4670,10 @@
       <c r="BB11" s="86"/>
       <c r="BC11" s="86"/>
       <c r="BD11" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BE11" s="72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BH11" s="51"/>
       <c r="BI11" s="51"/>
@@ -4674,7 +4681,7 @@
       <c r="BK11" s="51"/>
       <c r="BL11" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="12" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="12" s="88">
       <c r="A12" s="67"/>
       <c r="B12" s="68" t="n">
         <v>1501016</v>
@@ -4683,7 +4690,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="69" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E12" s="69" t="s">
         <v>80</v>
@@ -4702,7 +4709,7 @@
       </c>
       <c r="J12" s="70"/>
       <c r="K12" s="69" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L12" s="71" t="n">
         <v>0</v>
@@ -4712,7 +4719,7 @@
       </c>
       <c r="N12" s="73"/>
       <c r="O12" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P12" s="75" t="n">
         <v>27</v>
@@ -4722,16 +4729,16 @@
       </c>
       <c r="R12" s="75"/>
       <c r="S12" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T12" s="76" t="n">
         <v>1</v>
       </c>
       <c r="U12" s="77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V12" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W12" s="78"/>
       <c r="X12" s="77"/>
@@ -4747,13 +4754,13 @@
         <v>11</v>
       </c>
       <c r="AD12" s="81" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE12" s="80" t="n">
         <v>4</v>
       </c>
       <c r="AF12" s="81" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AG12" s="82"/>
       <c r="AH12" s="82"/>
@@ -4779,10 +4786,10 @@
       <c r="BB12" s="86"/>
       <c r="BC12" s="86"/>
       <c r="BD12" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BE12" s="72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BH12" s="51"/>
       <c r="BI12" s="51"/>
@@ -4790,7 +4797,7 @@
       <c r="BK12" s="51"/>
       <c r="BL12" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="13" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="13" s="88">
       <c r="A13" s="67"/>
       <c r="B13" s="68" t="n">
         <v>1501016</v>
@@ -4799,7 +4806,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="69" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E13" s="69" t="s">
         <v>80</v>
@@ -4818,7 +4825,7 @@
       </c>
       <c r="J13" s="70"/>
       <c r="K13" s="69" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L13" s="71" t="n">
         <v>0</v>
@@ -4828,7 +4835,7 @@
       </c>
       <c r="N13" s="73"/>
       <c r="O13" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P13" s="75" t="n">
         <v>27</v>
@@ -4838,16 +4845,16 @@
       </c>
       <c r="R13" s="75"/>
       <c r="S13" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T13" s="76" t="n">
         <v>401</v>
       </c>
       <c r="U13" s="77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V13" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W13" s="78"/>
       <c r="X13" s="77"/>
@@ -4863,13 +4870,13 @@
         <v>5</v>
       </c>
       <c r="AD13" s="81" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE13" s="80" t="n">
         <v>4</v>
       </c>
       <c r="AF13" s="81" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AG13" s="82"/>
       <c r="AH13" s="82"/>
@@ -4895,10 +4902,10 @@
       <c r="BB13" s="86"/>
       <c r="BC13" s="86"/>
       <c r="BD13" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BE13" s="72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BH13" s="51"/>
       <c r="BI13" s="51"/>
@@ -4906,7 +4913,7 @@
       <c r="BK13" s="51"/>
       <c r="BL13" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="14" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="14" s="88">
       <c r="A14" s="67"/>
       <c r="B14" s="68" t="n">
         <v>1501016</v>
@@ -4915,7 +4922,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="69" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E14" s="69" t="s">
         <v>80</v>
@@ -4934,7 +4941,7 @@
       </c>
       <c r="J14" s="70"/>
       <c r="K14" s="69" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L14" s="71" t="n">
         <v>0</v>
@@ -4944,7 +4951,7 @@
       </c>
       <c r="N14" s="73"/>
       <c r="O14" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P14" s="75" t="n">
         <v>27</v>
@@ -4954,16 +4961,16 @@
       </c>
       <c r="R14" s="75"/>
       <c r="S14" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T14" s="76" t="n">
         <v>1</v>
       </c>
       <c r="U14" s="77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V14" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W14" s="78"/>
       <c r="X14" s="77"/>
@@ -4979,13 +4986,13 @@
         <v>7</v>
       </c>
       <c r="AD14" s="81" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE14" s="80" t="n">
         <v>4</v>
       </c>
       <c r="AF14" s="81" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AG14" s="82"/>
       <c r="AH14" s="82"/>
@@ -5011,10 +5018,10 @@
       <c r="BB14" s="86"/>
       <c r="BC14" s="86"/>
       <c r="BD14" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BE14" s="72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BH14" s="51"/>
       <c r="BI14" s="51"/>
@@ -5022,7 +5029,7 @@
       <c r="BK14" s="51"/>
       <c r="BL14" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="15" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="15" s="88">
       <c r="A15" s="67"/>
       <c r="B15" s="68" t="n">
         <v>1501016</v>
@@ -5031,7 +5038,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="69" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E15" s="69" t="s">
         <v>80</v>
@@ -5050,7 +5057,7 @@
       </c>
       <c r="J15" s="70"/>
       <c r="K15" s="69" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L15" s="71" t="n">
         <v>0</v>
@@ -5060,7 +5067,7 @@
       </c>
       <c r="N15" s="73"/>
       <c r="O15" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P15" s="75" t="n">
         <v>27</v>
@@ -5070,16 +5077,16 @@
       </c>
       <c r="R15" s="75"/>
       <c r="S15" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T15" s="76" t="n">
         <v>1</v>
       </c>
       <c r="U15" s="77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V15" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W15" s="78"/>
       <c r="X15" s="77"/>
@@ -5095,13 +5102,13 @@
         <v>8</v>
       </c>
       <c r="AD15" s="81" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE15" s="80" t="n">
         <v>4</v>
       </c>
       <c r="AF15" s="81" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AG15" s="82"/>
       <c r="AH15" s="82"/>
@@ -5127,10 +5134,10 @@
       <c r="BB15" s="86"/>
       <c r="BC15" s="86"/>
       <c r="BD15" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BE15" s="72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BH15" s="51"/>
       <c r="BI15" s="51"/>
@@ -5138,7 +5145,7 @@
       <c r="BK15" s="51"/>
       <c r="BL15" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="16" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16" s="88">
       <c r="A16" s="67"/>
       <c r="B16" s="68" t="n">
         <v>1501016</v>
@@ -5147,7 +5154,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="69" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E16" s="69" t="s">
         <v>80</v>
@@ -5166,7 +5173,7 @@
       </c>
       <c r="J16" s="70"/>
       <c r="K16" s="69" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="L16" s="71" t="n">
         <v>0</v>
@@ -5176,7 +5183,7 @@
       </c>
       <c r="N16" s="73"/>
       <c r="O16" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P16" s="75" t="n">
         <v>27</v>
@@ -5186,19 +5193,19 @@
       </c>
       <c r="R16" s="75"/>
       <c r="S16" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T16" s="76" t="n">
         <v>401</v>
       </c>
       <c r="U16" s="77" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="V16" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W16" s="78" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="X16" s="77" t="n">
         <v>0</v>
@@ -5246,7 +5253,7 @@
       <c r="BK16" s="51"/>
       <c r="BL16" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="17" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17" s="88">
       <c r="A17" s="67"/>
       <c r="B17" s="68" t="n">
         <v>1501016</v>
@@ -5255,7 +5262,7 @@
         <v>11</v>
       </c>
       <c r="D17" s="69" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E17" s="69" t="s">
         <v>80</v>
@@ -5274,7 +5281,7 @@
       </c>
       <c r="J17" s="70"/>
       <c r="K17" s="69" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L17" s="71" t="n">
         <v>0</v>
@@ -5284,7 +5291,7 @@
       </c>
       <c r="N17" s="73"/>
       <c r="O17" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P17" s="75" t="n">
         <v>27</v>
@@ -5294,19 +5301,19 @@
       </c>
       <c r="R17" s="75"/>
       <c r="S17" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T17" s="76" t="n">
         <v>1</v>
       </c>
       <c r="U17" s="77" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="V17" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W17" s="78" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="X17" s="77" t="n">
         <v>0</v>
@@ -5354,7 +5361,7 @@
       <c r="BK17" s="51"/>
       <c r="BL17" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="18" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18" s="88">
       <c r="A18" s="67"/>
       <c r="B18" s="68" t="n">
         <v>1501016</v>
@@ -5363,7 +5370,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="69" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E18" s="69" t="s">
         <v>80</v>
@@ -5382,7 +5389,7 @@
       </c>
       <c r="J18" s="70"/>
       <c r="K18" s="69" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L18" s="71" t="n">
         <v>0</v>
@@ -5392,7 +5399,7 @@
       </c>
       <c r="N18" s="73"/>
       <c r="O18" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P18" s="75" t="n">
         <v>27</v>
@@ -5402,19 +5409,19 @@
       </c>
       <c r="R18" s="75"/>
       <c r="S18" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T18" s="76" t="n">
         <v>1</v>
       </c>
       <c r="U18" s="77" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="V18" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W18" s="78" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="X18" s="77" t="n">
         <v>0</v>
@@ -5462,7 +5469,7 @@
       <c r="BK18" s="51"/>
       <c r="BL18" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="19" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="19" s="88">
       <c r="A19" s="67"/>
       <c r="B19" s="68" t="n">
         <v>1501016</v>
@@ -5471,7 +5478,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="69" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E19" s="69" t="s">
         <v>80</v>
@@ -5490,7 +5497,7 @@
       </c>
       <c r="J19" s="70"/>
       <c r="K19" s="69" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L19" s="71" t="n">
         <v>0</v>
@@ -5500,7 +5507,7 @@
       </c>
       <c r="N19" s="73"/>
       <c r="O19" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P19" s="75" t="n">
         <v>27</v>
@@ -5510,16 +5517,16 @@
       </c>
       <c r="R19" s="75"/>
       <c r="S19" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T19" s="76" t="n">
         <v>401</v>
       </c>
       <c r="U19" s="77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V19" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W19" s="78"/>
       <c r="X19" s="77"/>
@@ -5535,13 +5542,13 @@
         <v>4</v>
       </c>
       <c r="AD19" s="81" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE19" s="80" t="n">
         <v>4</v>
       </c>
       <c r="AF19" s="81" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AG19" s="82"/>
       <c r="AH19" s="82"/>
@@ -5567,10 +5574,10 @@
       <c r="BB19" s="86"/>
       <c r="BC19" s="86"/>
       <c r="BD19" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BE19" s="72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BH19" s="51"/>
       <c r="BI19" s="51"/>
@@ -5578,7 +5585,7 @@
       <c r="BK19" s="51"/>
       <c r="BL19" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="20" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="20" s="88">
       <c r="A20" s="67"/>
       <c r="B20" s="68" t="n">
         <v>1501016</v>
@@ -5587,7 +5594,7 @@
         <v>14</v>
       </c>
       <c r="D20" s="69" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E20" s="69" t="s">
         <v>80</v>
@@ -5606,7 +5613,7 @@
       </c>
       <c r="J20" s="70"/>
       <c r="K20" s="69" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L20" s="71" t="n">
         <v>0</v>
@@ -5616,7 +5623,7 @@
       </c>
       <c r="N20" s="73"/>
       <c r="O20" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P20" s="75" t="n">
         <v>27</v>
@@ -5626,16 +5633,16 @@
       </c>
       <c r="R20" s="75"/>
       <c r="S20" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T20" s="76" t="n">
         <v>1</v>
       </c>
       <c r="U20" s="77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V20" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W20" s="78"/>
       <c r="X20" s="77"/>
@@ -5651,13 +5658,13 @@
         <v>6</v>
       </c>
       <c r="AD20" s="81" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE20" s="80" t="n">
         <v>4</v>
       </c>
       <c r="AF20" s="81" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AG20" s="82"/>
       <c r="AH20" s="82"/>
@@ -5683,10 +5690,10 @@
       <c r="BB20" s="86"/>
       <c r="BC20" s="86"/>
       <c r="BD20" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BE20" s="72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BH20" s="51"/>
       <c r="BI20" s="51"/>
@@ -5694,7 +5701,7 @@
       <c r="BK20" s="51"/>
       <c r="BL20" s="51"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="21" s="88">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="21" s="88">
       <c r="A21" s="67"/>
       <c r="B21" s="68" t="n">
         <v>1501016</v>
@@ -5703,7 +5710,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="69" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E21" s="69" t="s">
         <v>80</v>
@@ -5722,7 +5729,7 @@
       </c>
       <c r="J21" s="70"/>
       <c r="K21" s="69" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L21" s="71" t="n">
         <v>0</v>
@@ -5732,7 +5739,7 @@
       </c>
       <c r="N21" s="73"/>
       <c r="O21" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P21" s="75" t="n">
         <v>27</v>
@@ -5742,16 +5749,16 @@
       </c>
       <c r="R21" s="75"/>
       <c r="S21" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T21" s="76" t="n">
         <v>1</v>
       </c>
       <c r="U21" s="77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V21" s="77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W21" s="78"/>
       <c r="X21" s="77"/>
@@ -5767,13 +5774,13 @@
         <v>5</v>
       </c>
       <c r="AD21" s="81" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE21" s="80" t="n">
         <v>4</v>
       </c>
       <c r="AF21" s="81" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AG21" s="82"/>
       <c r="AH21" s="82"/>
@@ -5799,10 +5806,10 @@
       <c r="BB21" s="86"/>
       <c r="BC21" s="86"/>
       <c r="BD21" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BE21" s="72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BH21" s="51"/>
       <c r="BI21" s="51"/>
@@ -7299,7 +7306,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="43">
       <c r="B43" s="111" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C43" s="111"/>
       <c r="D43" s="112"/>
@@ -7359,7 +7366,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="44">
       <c r="B44" s="115" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C44" s="115"/>
       <c r="D44" s="112"/>
@@ -7392,7 +7399,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="45">
       <c r="B45" s="118" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C45" s="118"/>
       <c r="D45" s="112"/>
@@ -7445,7 +7452,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="46">
       <c r="B46" s="119" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C46" s="119"/>
       <c r="D46" s="112"/>
@@ -7498,7 +7505,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="47">
       <c r="B47" s="120" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C47" s="120"/>
       <c r="D47" s="112"/>
@@ -7552,7 +7559,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="48">
       <c r="B48" s="121" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C48" s="121"/>
       <c r="D48" s="112"/>
@@ -7606,7 +7613,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="49">
       <c r="B49" s="122" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C49" s="122"/>
       <c r="D49" s="112"/>
@@ -7660,7 +7667,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="50">
       <c r="B50" s="123" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C50" s="123"/>
       <c r="D50" s="112"/>
@@ -7764,7 +7771,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="52">
       <c r="B52" s="124"/>
       <c r="C52" s="111" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D52" s="111"/>
       <c r="E52" s="13"/>
@@ -7818,7 +7825,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="53">
       <c r="B53" s="125"/>
       <c r="C53" s="111" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D53" s="111"/>
       <c r="E53" s="13"/>
@@ -7872,7 +7879,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="54">
       <c r="B54" s="126"/>
       <c r="C54" s="111" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D54" s="111"/>
       <c r="E54" s="13"/>
@@ -8158,19 +8165,9 @@
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="C54:D54"/>
   </mergeCells>
-  <conditionalFormatting sqref="BE22:BE39,BE8:BE17">
+  <conditionalFormatting sqref="BE8:BE39">
     <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
-      <formula>IF(N8=2,1,0)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BE18">
-    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="3" rank="0" text="" type="expression">
-      <formula>IF(N18=2,1,0)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BE19:BE21">
-    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="4" rank="0" text="" type="expression">
-      <formula>IF(N19=2,1,0)</formula>
+      <formula>IF(#REF!=2,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="28">
@@ -8312,8 +8309,8 @@
   </sheetPr>
   <dimension ref="A1:D9999"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="A2" activeCellId="1" pane="topLeft" sqref="R8 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8327,58 +8324,58 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="1">
       <c r="A1" s="134" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B1" s="135" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C1" s="134" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D1" s="134" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="2">
       <c r="A2" s="132" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B2" s="136" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C2" s="132" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D2" s="132" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="3">
       <c r="A3" s="132" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="136" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="132" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="132" t="s">
         <v>149</v>
-      </c>
-      <c r="B3" s="136" t="s">
-        <v>150</v>
-      </c>
-      <c r="C3" s="132" t="s">
-        <v>147</v>
-      </c>
-      <c r="D3" s="132" t="s">
-        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="9999">
       <c r="A9999" s="132" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B9999" s="136" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C9999" s="132" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D9999" s="132" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -8399,8 +8396,8 @@
   </sheetPr>
   <dimension ref="A1:BG37"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="N1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N8" activeCellId="0" pane="topLeft" sqref="N8"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="N1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="N8" activeCellId="1" pane="topLeft" sqref="R8 N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8454,15 +8451,15 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="1">
       <c r="A1" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="137"/>
       <c r="D1" s="138" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E1" s="139" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F1" s="139"/>
       <c r="G1" s="139"/>
@@ -8688,10 +8685,10 @@
         <v>25</v>
       </c>
       <c r="P4" s="153" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="Q4" s="153" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="R4" s="153" t="s">
         <v>27</v>
@@ -8712,7 +8709,7 @@
       <c r="X4" s="155"/>
       <c r="Y4" s="155"/>
       <c r="Z4" s="156" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AA4" s="156"/>
       <c r="AB4" s="156"/>
@@ -8720,7 +8717,7 @@
       <c r="AD4" s="156"/>
       <c r="AE4" s="156"/>
       <c r="AF4" s="155" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AG4" s="155"/>
       <c r="AH4" s="155" t="s">
@@ -8898,46 +8895,46 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="6.75" outlineLevel="0" r="7" s="172">
       <c r="A7" s="163" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B7" s="164" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C7" s="165" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D7" s="163" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E7" s="163" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F7" s="166"/>
       <c r="G7" s="163" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H7" s="167"/>
       <c r="I7" s="167"/>
       <c r="J7" s="164" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K7" s="168"/>
       <c r="L7" s="168"/>
       <c r="M7" s="166"/>
       <c r="N7" s="165" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="O7" s="163" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="P7" s="163" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="Q7" s="166"/>
       <c r="R7" s="166"/>
       <c r="S7" s="169"/>
       <c r="T7" s="170" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U7" s="171"/>
       <c r="V7" s="166"/>
@@ -8975,28 +8972,28 @@
         <v>1</v>
       </c>
       <c r="C8" s="173" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D8" s="174" t="s">
         <v>80</v>
       </c>
       <c r="E8" s="174" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F8" s="174" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G8" s="175" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H8" s="175" t="n">
         <v>29161</v>
       </c>
       <c r="I8" s="175" t="s">
+        <v>166</v>
+      </c>
+      <c r="J8" s="176" t="s">
         <v>165</v>
-      </c>
-      <c r="J8" s="176" t="s">
-        <v>164</v>
       </c>
       <c r="K8" s="177" t="n">
         <v>1</v>
@@ -9006,7 +9003,7 @@
       </c>
       <c r="M8" s="179"/>
       <c r="N8" s="180" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O8" s="181" t="n">
         <v>1</v>
@@ -9015,16 +9012,16 @@
         <v>3122</v>
       </c>
       <c r="Q8" s="181" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="R8" s="181" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="S8" s="182" t="n">
         <v>0</v>
       </c>
       <c r="T8" s="183" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="U8" s="183" t="str">
         <f aca="false">IF(LEN(T8)=0,"",IF(ISERROR(SEARCH("APIMMD",$T8)),IF(MID(T8,1,3)="PLC","X",""),"X"))</f>
@@ -9071,28 +9068,28 @@
         <v>2</v>
       </c>
       <c r="C9" s="173" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D9" s="174" t="s">
         <v>80</v>
       </c>
       <c r="E9" s="174" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F9" s="174" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G9" s="175" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H9" s="175" t="n">
         <v>29161</v>
       </c>
       <c r="I9" s="175" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J9" s="176" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K9" s="177" t="n">
         <v>1</v>
@@ -9102,7 +9099,7 @@
       </c>
       <c r="M9" s="179"/>
       <c r="N9" s="180" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O9" s="181" t="n">
         <v>1</v>
@@ -9111,16 +9108,16 @@
         <v>3122</v>
       </c>
       <c r="Q9" s="181" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="R9" s="181" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="S9" s="182" t="n">
         <v>0</v>
       </c>
       <c r="T9" s="183" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="U9" s="183" t="str">
         <f aca="false">IF(LEN(T9)=0,"",IF(ISERROR(SEARCH("APIMMD",$T9)),IF(MID(T9,1,3)="PLC","X",""),"X"))</f>
@@ -9167,16 +9164,16 @@
         <v>3</v>
       </c>
       <c r="C10" s="173" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D10" s="174" t="s">
         <v>80</v>
       </c>
       <c r="E10" s="174" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F10" s="174" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G10" s="175" t="s">
         <v>82</v>
@@ -9185,7 +9182,7 @@
         <v>31169</v>
       </c>
       <c r="I10" s="175" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J10" s="176" t="s">
         <v>82</v>
@@ -9198,7 +9195,7 @@
       </c>
       <c r="M10" s="179"/>
       <c r="N10" s="180" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O10" s="181" t="n">
         <v>28</v>
@@ -9208,13 +9205,13 @@
       </c>
       <c r="Q10" s="181"/>
       <c r="R10" s="181" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S10" s="182" t="n">
         <v>10</v>
       </c>
       <c r="T10" s="183" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="U10" s="183" t="str">
         <f aca="false">IF(LEN(T10)=0,"",IF(ISERROR(SEARCH("APIMMD",$T10)),IF(MID(T10,1,3)="PLC","X",""),"X"))</f>
@@ -9261,16 +9258,16 @@
         <v>4</v>
       </c>
       <c r="C11" s="173" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D11" s="174" t="s">
         <v>80</v>
       </c>
       <c r="E11" s="174" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F11" s="174" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G11" s="175" t="s">
         <v>82</v>
@@ -9279,10 +9276,10 @@
         <v>31169</v>
       </c>
       <c r="I11" s="175" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J11" s="176" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K11" s="177" t="n">
         <v>1</v>
@@ -9292,7 +9289,7 @@
       </c>
       <c r="M11" s="179"/>
       <c r="N11" s="180" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O11" s="181" t="n">
         <v>28</v>
@@ -9302,13 +9299,13 @@
       </c>
       <c r="Q11" s="181"/>
       <c r="R11" s="181" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S11" s="182" t="n">
         <v>10</v>
       </c>
       <c r="T11" s="183" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="U11" s="183" t="str">
         <f aca="false">IF(LEN(T11)=0,"",IF(ISERROR(SEARCH("APIMMD",$T11)),IF(MID(T11,1,3)="PLC","X",""),"X"))</f>
@@ -9355,24 +9352,24 @@
         <v>5</v>
       </c>
       <c r="C12" s="173" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D12" s="174" t="s">
         <v>80</v>
       </c>
       <c r="E12" s="174" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F12" s="174"/>
       <c r="G12" s="175" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H12" s="175"/>
       <c r="I12" s="175" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J12" s="176" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K12" s="177" t="n">
         <v>0</v>
@@ -9382,7 +9379,7 @@
       </c>
       <c r="M12" s="179"/>
       <c r="N12" s="180" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O12" s="181" t="n">
         <v>27</v>
@@ -9394,20 +9391,20 @@
         <v>171</v>
       </c>
       <c r="R12" s="181" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S12" s="182" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="T12" s="183" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="U12" s="183" t="str">
         <f aca="false">IF(LEN(T12)=0,"",IF(ISERROR(SEARCH("APIMMD",$T12)),IF(MID(T12,1,3)="PLC","X",""),"X"))</f>
         <v>X</v>
       </c>
       <c r="V12" s="184" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="W12" s="183" t="n">
         <v>0</v>
@@ -9449,26 +9446,26 @@
         <v>6</v>
       </c>
       <c r="C13" s="173" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D13" s="174" t="s">
         <v>80</v>
       </c>
       <c r="E13" s="174" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F13" s="174"/>
       <c r="G13" s="175" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H13" s="175" t="n">
         <v>399525</v>
       </c>
       <c r="I13" s="175" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J13" s="176" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K13" s="177" t="n">
         <v>0</v>
@@ -9478,7 +9475,7 @@
       </c>
       <c r="M13" s="179"/>
       <c r="N13" s="180" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O13" s="181" t="n">
         <v>27</v>
@@ -9490,13 +9487,13 @@
         <v>171</v>
       </c>
       <c r="R13" s="181" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S13" s="182" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="T13" s="183" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="U13" s="183" t="str">
         <f aca="false">IF(LEN(T13)=0,"",IF(ISERROR(SEARCH("APIMMD",$T13)),IF(MID(T13,1,3)="PLC","X",""),"X"))</f>
@@ -9507,7 +9504,7 @@
       <c r="X13" s="183"/>
       <c r="Y13" s="185"/>
       <c r="Z13" s="186" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AA13" s="186" t="n">
         <v>31</v>
@@ -9516,13 +9513,13 @@
         <v>2</v>
       </c>
       <c r="AC13" s="186" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AD13" s="186" t="n">
         <v>7</v>
       </c>
       <c r="AE13" s="186" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AF13" s="187"/>
       <c r="AG13" s="188"/>
@@ -9539,10 +9536,10 @@
       <c r="AR13" s="191"/>
       <c r="AS13" s="191"/>
       <c r="AT13" s="178" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AU13" s="178" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="14" s="192">
@@ -9553,24 +9550,24 @@
         <v>7</v>
       </c>
       <c r="C14" s="173" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D14" s="174" t="s">
         <v>80</v>
       </c>
       <c r="E14" s="174" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F14" s="174"/>
       <c r="G14" s="175" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H14" s="175" t="n">
         <v>38942</v>
       </c>
       <c r="I14" s="175"/>
       <c r="J14" s="176" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K14" s="177" t="n">
         <v>0</v>
@@ -9580,7 +9577,7 @@
       </c>
       <c r="M14" s="179"/>
       <c r="N14" s="180" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O14" s="181" t="n">
         <v>27</v>
@@ -9592,13 +9589,13 @@
         <v>171</v>
       </c>
       <c r="R14" s="181" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S14" s="182" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="T14" s="183" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="U14" s="183" t="str">
         <f aca="false">IF(LEN(T14)=0,"",IF(ISERROR(SEARCH("APIMMD",$T14)),IF(MID(T14,1,3)="PLC","X",""),"X"))</f>
@@ -9609,7 +9606,7 @@
       <c r="X14" s="183"/>
       <c r="Y14" s="185"/>
       <c r="Z14" s="186" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AA14" s="186" t="n">
         <v>31</v>
@@ -9618,13 +9615,13 @@
         <v>8</v>
       </c>
       <c r="AC14" s="186" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AD14" s="186" t="n">
         <v>7</v>
       </c>
       <c r="AE14" s="186" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AF14" s="187"/>
       <c r="AG14" s="188"/>
@@ -9641,10 +9638,10 @@
       <c r="AR14" s="191"/>
       <c r="AS14" s="191"/>
       <c r="AT14" s="178" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AU14" s="178" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="15" s="192">
@@ -9655,24 +9652,24 @@
         <v>8</v>
       </c>
       <c r="C15" s="173" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D15" s="174" t="s">
         <v>80</v>
       </c>
       <c r="E15" s="174" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F15" s="174"/>
       <c r="G15" s="175" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H15" s="175" t="n">
         <v>24990</v>
       </c>
       <c r="I15" s="175"/>
       <c r="J15" s="176" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K15" s="177" t="n">
         <v>0</v>
@@ -9682,7 +9679,7 @@
       </c>
       <c r="M15" s="179"/>
       <c r="N15" s="180" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O15" s="181" t="n">
         <v>24</v>
@@ -9695,7 +9692,7 @@
       <c r="S15" s="182"/>
       <c r="T15" s="183"/>
       <c r="U15" s="183" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="V15" s="184"/>
       <c r="W15" s="183"/>
@@ -10327,7 +10324,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="26">
       <c r="A26" s="111" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B26" s="111"/>
       <c r="C26" s="112"/>
@@ -10335,7 +10332,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="27">
       <c r="A27" s="115" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B27" s="115"/>
       <c r="C27" s="112"/>
@@ -10343,7 +10340,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="28">
       <c r="A28" s="118" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B28" s="118"/>
       <c r="C28" s="112"/>
@@ -10351,35 +10348,35 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="29">
       <c r="A29" s="119" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B29" s="119"/>
       <c r="C29" s="112"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="30">
       <c r="A30" s="120" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B30" s="120"/>
       <c r="C30" s="112"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="31">
       <c r="A31" s="121" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B31" s="121"/>
       <c r="C31" s="112"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="32">
       <c r="A32" s="122" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B32" s="122"/>
       <c r="C32" s="112"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="33">
       <c r="A33" s="123" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B33" s="123"/>
       <c r="C33" s="112"/>
@@ -10387,21 +10384,21 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="35">
       <c r="A35" s="124"/>
       <c r="B35" s="111" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C35" s="111"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="36">
       <c r="A36" s="125"/>
       <c r="B36" s="111" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C36" s="111"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="37">
       <c r="A37" s="126"/>
       <c r="B37" s="111" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C37" s="111"/>
     </row>
@@ -10592,8 +10589,8 @@
   </sheetPr>
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E36" activeCellId="0" pane="topLeft" sqref="E36"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="B56" activeCellId="1" pane="topLeft" sqref="R8 B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -10618,25 +10615,25 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="1">
       <c r="B1" s="202" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C1" s="203" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D1" s="203" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E1" s="202" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F1" s="202" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G1" s="204" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H1" s="205" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I1" s="206"/>
       <c r="J1" s="206"/>
@@ -10647,202 +10644,202 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="38.25" outlineLevel="0" r="2">
       <c r="A2" s="200" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B2" s="207" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C2" s="208" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D2" s="208"/>
       <c r="E2" s="207" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F2" s="207" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G2" s="209"/>
       <c r="H2" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="38.25" outlineLevel="0" r="3">
       <c r="A3" s="200" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B3" s="207" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="208" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D3" s="208"/>
       <c r="E3" s="207" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F3" s="207" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G3" s="209"/>
       <c r="H3" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="4">
       <c r="A4" s="200" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B4" s="210" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="211" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D4" s="211"/>
       <c r="E4" s="210" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F4" s="210" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G4" s="209" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H4" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="5">
       <c r="A5" s="200" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B5" s="212" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="213" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D5" s="213" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E5" s="214" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F5" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G5" s="209"/>
       <c r="H5" s="209" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>80</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
       <c r="A6" s="200" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B6" s="215" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C6" s="213" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D6" s="213"/>
       <c r="E6" s="214" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F6" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G6" s="209" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H6" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="7">
       <c r="A7" s="200" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B7" s="214" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C7" s="213"/>
       <c r="D7" s="213"/>
       <c r="E7" s="214" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F7" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G7" s="209" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H7" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="8">
       <c r="A8" s="200" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B8" s="214" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="213" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D8" s="213" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E8" s="214" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F8" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G8" s="209"/>
       <c r="H8" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.5" outlineLevel="0" r="9">
       <c r="A9" s="200" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B9" s="214" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C9" s="216" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D9" s="213" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E9" s="214" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F9" s="217" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G9" s="209"/>
       <c r="H9" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="10">
       <c r="A10" s="200" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B10" s="214" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C10" s="216"/>
       <c r="D10" s="213"/>
       <c r="E10" s="214" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F10" s="217"/>
       <c r="G10" s="209"/>
@@ -10850,29 +10847,29 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="11">
       <c r="A11" s="200" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B11" s="214" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="213" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D11" s="213"/>
       <c r="E11" s="214" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F11" s="214" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G11" s="209" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H11" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="12">
       <c r="A12" s="200" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B12" s="207" t="s">
         <v>45</v>
@@ -10880,34 +10877,34 @@
       <c r="C12" s="218"/>
       <c r="D12" s="218"/>
       <c r="E12" s="207" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F12" s="207" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G12" s="209"/>
       <c r="H12" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="13">
       <c r="A13" s="200" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B13" s="207" t="s">
         <v>46</v>
       </c>
       <c r="C13" s="218"/>
       <c r="D13" s="218" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E13" s="207" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F13" s="207" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G13" s="209"/>
       <c r="H13" s="209" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>0</v>
@@ -10924,7 +10921,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="14">
       <c r="A14" s="200" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B14" s="207" t="s">
         <v>23</v>
@@ -10932,103 +10929,103 @@
       <c r="C14" s="218"/>
       <c r="D14" s="218"/>
       <c r="E14" s="207" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F14" s="207" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G14" s="209" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H14" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="15">
       <c r="A15" s="200" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B15" s="214" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="213" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D15" s="213" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E15" s="214" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F15" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G15" s="209"/>
       <c r="H15" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="16">
       <c r="A16" s="200" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B16" s="214" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="213" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D16" s="213" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E16" s="214" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F16" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G16" s="209"/>
       <c r="H16" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="17">
       <c r="A17" s="200" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B17" s="214" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C17" s="213" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D17" s="213" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E17" s="214" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F17" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G17" s="209"/>
       <c r="H17" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="18">
       <c r="A18" s="200" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B18" s="214" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C18" s="213"/>
       <c r="D18" s="213"/>
       <c r="E18" s="214" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F18" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G18" s="209"/>
       <c r="H18" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="19">
       <c r="A19" s="200" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B19" s="214" t="s">
         <v>27</v>
@@ -11036,17 +11033,17 @@
       <c r="C19" s="213"/>
       <c r="D19" s="213"/>
       <c r="E19" s="214" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F19" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G19" s="209"/>
       <c r="H19" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="20">
       <c r="A20" s="200" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B20" s="214" t="s">
         <v>28</v>
@@ -11054,198 +11051,198 @@
       <c r="C20" s="213"/>
       <c r="D20" s="213"/>
       <c r="E20" s="214" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F20" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G20" s="209"/>
       <c r="H20" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="21">
       <c r="A21" s="200" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B21" s="207" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="218" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D21" s="218"/>
       <c r="E21" s="207" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F21" s="207" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G21" s="209"/>
       <c r="H21" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="22">
       <c r="A22" s="200" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B22" s="207" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="218"/>
       <c r="D22" s="218" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E22" s="207" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F22" s="207" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G22" s="209"/>
       <c r="H22" s="209" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="23">
       <c r="A23" s="200" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B23" s="207" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C23" s="218"/>
       <c r="D23" s="218" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E23" s="207" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F23" s="207" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G23" s="209"/>
       <c r="H23" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="24">
       <c r="A24" s="200" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B24" s="207" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C24" s="218"/>
       <c r="D24" s="218"/>
       <c r="E24" s="207" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F24" s="207" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G24" s="209"/>
       <c r="H24" s="209"/>
       <c r="I24" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="25">
       <c r="A25" s="200" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B25" s="207" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C25" s="218"/>
       <c r="D25" s="218"/>
       <c r="E25" s="207" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F25" s="207" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G25" s="209"/>
       <c r="H25" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="26">
       <c r="A26" s="200" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B26" s="207" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C26" s="218"/>
       <c r="D26" s="218"/>
       <c r="E26" s="207" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F26" s="207" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G26" s="209"/>
       <c r="H26" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="27">
       <c r="A27" s="200" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B27" s="207" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C27" s="218"/>
       <c r="D27" s="218"/>
       <c r="E27" s="207" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F27" s="207" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G27" s="209"/>
       <c r="H27" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="28">
       <c r="A28" s="200" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B28" s="207" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C28" s="218"/>
       <c r="D28" s="218"/>
       <c r="E28" s="207" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F28" s="207" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G28" s="209"/>
       <c r="H28" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="29">
       <c r="A29" s="200" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B29" s="207" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C29" s="218"/>
       <c r="D29" s="218"/>
       <c r="E29" s="207" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F29" s="207" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G29" s="209"/>
       <c r="H29" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="30">
       <c r="A30" s="200" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B30" s="207" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C30" s="218"/>
       <c r="D30" s="218"/>
       <c r="E30" s="207" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F30" s="207"/>
       <c r="G30" s="209"/>
@@ -11253,15 +11250,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="31">
       <c r="A31" s="200" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B31" s="207" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C31" s="218"/>
       <c r="D31" s="218"/>
       <c r="E31" s="207" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F31" s="207"/>
       <c r="G31" s="209"/>
@@ -11269,15 +11266,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="32">
       <c r="A32" s="200" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B32" s="207" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C32" s="218"/>
       <c r="D32" s="218"/>
       <c r="E32" s="207" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F32" s="207"/>
       <c r="G32" s="209"/>
@@ -11285,87 +11282,87 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="33">
       <c r="A33" s="200" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B33" s="207" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C33" s="218"/>
       <c r="D33" s="218"/>
       <c r="E33" s="207" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F33" s="207" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G33" s="209"/>
       <c r="H33" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="34">
       <c r="A34" s="200" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B34" s="207" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C34" s="218"/>
       <c r="D34" s="218"/>
       <c r="E34" s="207" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F34" s="207" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G34" s="209"/>
       <c r="H34" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="35">
       <c r="A35" s="200" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B35" s="207" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C35" s="218"/>
       <c r="D35" s="218"/>
       <c r="E35" s="207" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F35" s="207" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G35" s="209"/>
       <c r="H35" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="36">
       <c r="A36" s="200" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B36" s="207" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C36" s="218"/>
       <c r="D36" s="218"/>
       <c r="E36" s="207" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F36" s="207" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G36" s="209"/>
       <c r="H36" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="37">
       <c r="A37" s="200" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B37" s="207" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C37" s="218"/>
       <c r="D37" s="218"/>
       <c r="E37" s="207" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F37" s="207"/>
       <c r="G37" s="209"/>
@@ -11373,15 +11370,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="38">
       <c r="A38" s="200" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B38" s="207" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C38" s="218"/>
       <c r="D38" s="218"/>
       <c r="E38" s="207" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F38" s="207"/>
       <c r="G38" s="209"/>
@@ -11389,15 +11386,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="39">
       <c r="A39" s="200" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B39" s="207" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C39" s="218"/>
       <c r="D39" s="218"/>
       <c r="E39" s="207" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F39" s="207"/>
       <c r="G39" s="209"/>
@@ -11405,15 +11402,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="40">
       <c r="A40" s="200" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B40" s="207" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C40" s="218"/>
       <c r="D40" s="218"/>
       <c r="E40" s="207" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F40" s="207"/>
       <c r="G40" s="209"/>
@@ -11421,43 +11418,43 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="41">
       <c r="A41" s="200" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B41" s="214" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C41" s="213"/>
       <c r="D41" s="213"/>
       <c r="E41" s="214" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="F41" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G41" s="209"/>
       <c r="H41" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="42">
       <c r="A42" s="200" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B42" s="214" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C42" s="213"/>
       <c r="D42" s="213"/>
       <c r="E42" s="214" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="F42" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G42" s="209"/>
       <c r="H42" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="43">
       <c r="A43" s="200" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B43" s="214" t="s">
         <v>72</v>
@@ -11465,17 +11462,17 @@
       <c r="C43" s="213"/>
       <c r="D43" s="213"/>
       <c r="E43" s="214" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="F43" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G43" s="209"/>
       <c r="H43" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="44">
       <c r="A44" s="200" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B44" s="214" t="s">
         <v>73</v>
@@ -11483,53 +11480,53 @@
       <c r="C44" s="213"/>
       <c r="D44" s="213"/>
       <c r="E44" s="214" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F44" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G44" s="209"/>
       <c r="H44" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="45">
       <c r="A45" s="200" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B45" s="214" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C45" s="213"/>
       <c r="D45" s="213"/>
       <c r="E45" s="214" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="F45" s="214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G45" s="209"/>
       <c r="H45" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.5" outlineLevel="0" r="46">
       <c r="A46" s="200" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B46" s="219" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C46" s="220"/>
       <c r="D46" s="220"/>
       <c r="E46" s="219" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F46" s="219" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G46" s="209"/>
       <c r="H46" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="47">
       <c r="A47" s="200" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B47" s="214" t="s">
         <v>41</v>
@@ -11537,17 +11534,17 @@
       <c r="C47" s="213"/>
       <c r="D47" s="213"/>
       <c r="E47" s="214" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="F47" s="214"/>
       <c r="G47" s="209" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H47" s="209"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.25" outlineLevel="0" r="48">
       <c r="A48" s="200" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B48" s="214" t="s">
         <v>42</v>
@@ -11555,11 +11552,11 @@
       <c r="C48" s="213"/>
       <c r="D48" s="213"/>
       <c r="E48" s="214" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F48" s="214"/>
       <c r="G48" s="221" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H48" s="221"/>
     </row>
@@ -11594,8 +11591,8 @@
   </sheetPr>
   <dimension ref="A1:M131"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A94" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B8" activeCellId="0" pane="topLeft" sqref="B8"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="B8" activeCellId="1" pane="topLeft" sqref="R8 B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -11614,7 +11611,7 @@
       <c r="B1" s="227"/>
       <c r="C1" s="131"/>
       <c r="D1" s="228" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E1" s="228"/>
       <c r="F1" s="229"/>
@@ -11623,68 +11620,68 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="2">
       <c r="A2" s="230" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B2" s="231" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="131"/>
       <c r="D2" s="232" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E2" s="232"/>
       <c r="F2" s="233" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="G2" s="131"/>
       <c r="H2" s="131"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="3">
       <c r="A3" s="234" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B3" s="235" t="n">
         <v>8</v>
       </c>
       <c r="C3" s="131"/>
       <c r="D3" s="232" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E3" s="232"/>
       <c r="F3" s="236" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="G3" s="131"/>
       <c r="H3" s="131"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="4">
       <c r="A4" s="230" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B4" s="231" t="n">
         <v>66</v>
       </c>
       <c r="C4" s="131"/>
       <c r="D4" s="232" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E4" s="232"/>
       <c r="F4" s="236" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="G4" s="131"/>
       <c r="H4" s="131"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="5">
       <c r="A5" s="230" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B5" s="231" t="n">
         <v>5</v>
       </c>
       <c r="C5" s="131"/>
       <c r="D5" s="232" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E5" s="232"/>
       <c r="F5" s="237" t="n">
@@ -11695,43 +11692,43 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
       <c r="A6" s="230" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B6" s="231" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="131"/>
       <c r="D6" s="232" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E6" s="232"/>
       <c r="F6" s="236" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G6" s="131"/>
       <c r="H6" s="131"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="7">
       <c r="A7" s="230" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B7" s="238" t="n">
         <v>-1</v>
       </c>
       <c r="C7" s="131"/>
       <c r="D7" s="232" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E7" s="232"/>
       <c r="F7" s="236" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="G7" s="131"/>
       <c r="H7" s="131"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="8">
       <c r="A8" s="230" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B8" s="238" t="n">
         <v>1</v>
@@ -11745,10 +11742,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="9">
       <c r="A9" s="230" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B9" s="231" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C9" s="131"/>
       <c r="D9" s="131"/>
@@ -11759,10 +11756,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="10">
       <c r="A10" s="230" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B10" s="231" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C10" s="131"/>
       <c r="D10" s="131"/>
@@ -11773,10 +11770,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="11">
       <c r="A11" s="230" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B11" s="231" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C11" s="131"/>
       <c r="D11" s="239"/>
@@ -11787,10 +11784,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="12">
       <c r="A12" s="230" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B12" s="231" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C12" s="131"/>
       <c r="D12" s="131"/>
@@ -11801,10 +11798,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="13">
       <c r="A13" s="230" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B13" s="238" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C13" s="131"/>
       <c r="D13" s="131"/>
@@ -11815,7 +11812,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="14">
       <c r="A14" s="240" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B14" s="241" t="n">
         <v>4</v>
@@ -11829,7 +11826,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="15">
       <c r="A15" s="240" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B15" s="241" t="n">
         <v>6</v>
@@ -11843,10 +11840,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="16">
       <c r="A16" s="230" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B16" s="238" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C16" s="131"/>
       <c r="D16" s="131"/>
@@ -11867,13 +11864,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="18">
       <c r="A18" s="243" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B18" s="244" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C18" s="245" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D18" s="245"/>
       <c r="E18" s="131"/>
@@ -11883,13 +11880,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="19">
       <c r="A19" s="246" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B19" s="247" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C19" s="248" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D19" s="248"/>
       <c r="E19" s="131"/>
@@ -11899,13 +11896,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="20">
       <c r="A20" s="249" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B20" s="250" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C20" s="248" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D20" s="248"/>
       <c r="E20" s="131"/>
@@ -11915,13 +11912,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="21">
       <c r="A21" s="249" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B21" s="250" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C21" s="248" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D21" s="248"/>
       <c r="E21" s="131"/>
@@ -11931,13 +11928,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="22">
       <c r="A22" s="249" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B22" s="250" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C22" s="248" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D22" s="248"/>
       <c r="E22" s="131"/>
@@ -11947,13 +11944,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="23">
       <c r="A23" s="249" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B23" s="250" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C23" s="248" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D23" s="248"/>
       <c r="E23" s="131"/>
@@ -11963,13 +11960,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="24">
       <c r="A24" s="249" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B24" s="250" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C24" s="248" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D24" s="248"/>
       <c r="E24" s="131"/>
@@ -11979,13 +11976,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="25">
       <c r="A25" s="249" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B25" s="250" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C25" s="248" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D25" s="248"/>
       <c r="E25" s="131"/>
@@ -11995,13 +11992,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="26">
       <c r="A26" s="249" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B26" s="250" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C26" s="248" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D26" s="248"/>
       <c r="E26" s="131"/>
@@ -12031,13 +12028,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="29">
       <c r="A29" s="243" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B29" s="244" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C29" s="245" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D29" s="245"/>
       <c r="E29" s="131"/>
@@ -12047,13 +12044,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="30">
       <c r="A30" s="246" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B30" s="247" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C30" s="248" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D30" s="248"/>
       <c r="E30" s="131"/>
@@ -12063,13 +12060,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="31">
       <c r="A31" s="249" t="s">
+        <v>396</v>
+      </c>
+      <c r="B31" s="250" t="s">
+        <v>394</v>
+      </c>
+      <c r="C31" s="248" t="s">
         <v>395</v>
-      </c>
-      <c r="B31" s="250" t="s">
-        <v>393</v>
-      </c>
-      <c r="C31" s="248" t="s">
-        <v>394</v>
       </c>
       <c r="D31" s="248"/>
       <c r="E31" s="131"/>
@@ -12079,13 +12076,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="32">
       <c r="A32" s="249" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B32" s="250" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C32" s="248" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D32" s="248"/>
       <c r="E32" s="131"/>
@@ -12095,17 +12092,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="33">
       <c r="A33" s="249" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B33" s="250" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C33" s="248" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D33" s="248"/>
       <c r="E33" s="257" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F33" s="131"/>
       <c r="G33" s="131"/>
@@ -12133,13 +12130,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="36">
       <c r="A36" s="260" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B36" s="261" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C36" s="262" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D36" s="131"/>
       <c r="E36" s="131"/>
@@ -12149,7 +12146,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="37">
       <c r="A37" s="263" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B37" s="264" t="s">
         <v>13</v>
@@ -12165,7 +12162,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="38">
       <c r="A38" s="266" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B38" s="267" t="s">
         <v>14</v>
@@ -12181,7 +12178,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="39">
       <c r="A39" s="266" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B39" s="267" t="s">
         <v>15</v>
@@ -12197,7 +12194,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="40">
       <c r="A40" s="266" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B40" s="267" t="s">
         <v>16</v>
@@ -12213,7 +12210,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="41">
       <c r="A41" s="266" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B41" s="267" t="s">
         <v>17</v>
@@ -12229,10 +12226,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="42">
       <c r="A42" s="266" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B42" s="267" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C42" s="268" t="n">
         <v>7</v>
@@ -12245,10 +12242,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="43">
       <c r="A43" s="266" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B43" s="267" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C43" s="268" t="n">
         <v>8</v>
@@ -12261,10 +12258,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="44">
       <c r="A44" s="266" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B44" s="267" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C44" s="268" t="n">
         <v>9</v>
@@ -12278,7 +12275,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="45">
       <c r="A45" s="266"/>
       <c r="B45" s="267" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C45" s="268" t="n">
         <v>10</v>
@@ -12291,7 +12288,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="46">
       <c r="A46" s="266" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B46" s="267" t="s">
         <v>21</v>
@@ -12308,7 +12305,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="47">
       <c r="A47" s="266"/>
       <c r="B47" s="267" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C47" s="268" t="n">
         <v>12</v>
@@ -12321,10 +12318,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="48">
       <c r="A48" s="266" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B48" s="267" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C48" s="268" t="n">
         <v>13</v>
@@ -12342,7 +12339,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="49">
       <c r="A49" s="266"/>
       <c r="B49" s="267" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C49" s="268" t="n">
         <v>14</v>
@@ -12369,7 +12366,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="51">
       <c r="A51" s="266" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B51" s="267" t="s">
         <v>25</v>
@@ -12385,10 +12382,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="52">
       <c r="A52" s="266" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B52" s="267" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C52" s="268" t="n">
         <v>17</v>
@@ -12401,10 +12398,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="53">
       <c r="A53" s="266" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B53" s="267" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C53" s="268" t="n">
         <v>18</v>
@@ -12417,7 +12414,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="54">
       <c r="A54" s="266" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B54" s="267" t="s">
         <v>27</v>
@@ -12433,7 +12430,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="55">
       <c r="A55" s="266" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B55" s="267" t="s">
         <v>28</v>
@@ -12463,7 +12460,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="57">
       <c r="A57" s="266" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B57" s="267" t="s">
         <v>30</v>
@@ -12479,10 +12476,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="58">
       <c r="A58" s="266" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B58" s="270" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C58" s="271" t="n">
         <v>23</v>
@@ -12495,10 +12492,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="59">
       <c r="A59" s="266" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B59" s="270" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C59" s="271" t="n">
         <v>24</v>
@@ -12511,10 +12508,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="60">
       <c r="A60" s="266" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B60" s="270" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C60" s="271" t="n">
         <v>25</v>
@@ -12527,10 +12524,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="61">
       <c r="A61" s="266" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B61" s="270" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C61" s="271" t="n">
         <v>26</v>
@@ -12543,10 +12540,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="62">
       <c r="A62" s="266" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B62" s="272" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C62" s="273" t="n">
         <v>27</v>
@@ -12559,10 +12556,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="63">
       <c r="A63" s="266" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B63" s="272" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C63" s="273" t="n">
         <v>28</v>
@@ -12575,10 +12572,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="64">
       <c r="A64" s="266" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B64" s="272" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C64" s="273" t="n">
         <v>29</v>
@@ -12591,10 +12588,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="65">
       <c r="A65" s="266" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B65" s="272" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C65" s="273" t="n">
         <v>30</v>
@@ -12608,7 +12605,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="66">
       <c r="A66" s="274"/>
       <c r="B66" s="272" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C66" s="273" t="n">
         <v>31</v>
@@ -12622,7 +12619,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="67">
       <c r="A67" s="274"/>
       <c r="B67" s="272" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C67" s="273" t="n">
         <v>32</v>
@@ -12635,10 +12632,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="68">
       <c r="A68" s="266" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B68" s="275" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C68" s="276" t="n">
         <v>33</v>
@@ -12651,10 +12648,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="69">
       <c r="A69" s="266" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B69" s="275" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C69" s="276" t="n">
         <v>34</v>
@@ -12667,10 +12664,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="70">
       <c r="A70" s="266" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B70" s="277" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C70" s="278" t="n">
         <v>35</v>
@@ -12683,10 +12680,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="71">
       <c r="A71" s="266" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B71" s="277" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C71" s="278" t="n">
         <v>36</v>
@@ -12699,10 +12696,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="72">
       <c r="A72" s="266" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B72" s="279" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C72" s="280" t="n">
         <v>37</v>
@@ -12715,10 +12712,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="73">
       <c r="A73" s="266" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B73" s="279" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C73" s="280" t="n">
         <v>38</v>
@@ -12731,10 +12728,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="74">
       <c r="A74" s="266" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B74" s="279" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C74" s="280" t="n">
         <v>39</v>
@@ -12747,10 +12744,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="75">
       <c r="A75" s="266" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B75" s="279" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C75" s="280" t="n">
         <v>40</v>
@@ -12763,10 +12760,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="76">
       <c r="A76" s="266" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B76" s="279" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C76" s="280" t="n">
         <v>41</v>
@@ -12779,10 +12776,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="77">
       <c r="A77" s="266" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B77" s="281" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C77" s="282" t="n">
         <v>42</v>
@@ -12795,10 +12792,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="78">
       <c r="A78" s="266" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B78" s="281" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C78" s="282" t="n">
         <v>43</v>
@@ -12811,10 +12808,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="79">
       <c r="A79" s="266" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B79" s="281" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C79" s="282" t="n">
         <v>44</v>
@@ -12827,10 +12824,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="80">
       <c r="A80" s="266" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B80" s="281" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C80" s="282" t="n">
         <v>45</v>
@@ -12843,10 +12840,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="81">
       <c r="A81" s="266" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B81" s="283" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C81" s="284" t="n">
         <v>46</v>
@@ -12859,10 +12856,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="82">
       <c r="A82" s="266" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B82" s="283" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C82" s="284" t="n">
         <v>47</v>
@@ -12875,10 +12872,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="83">
       <c r="A83" s="266" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B83" s="283" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C83" s="284" t="n">
         <v>48</v>
@@ -12891,10 +12888,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.5" outlineLevel="0" r="84">
       <c r="A84" s="266" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B84" s="283" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C84" s="284" t="n">
         <v>49</v>
@@ -12907,10 +12904,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="85">
       <c r="A85" s="266" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B85" s="285" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C85" s="286" t="n">
         <v>50</v>
@@ -12923,10 +12920,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="86">
       <c r="A86" s="266" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B86" s="285" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C86" s="286" t="n">
         <v>51</v>
@@ -12939,10 +12936,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="87">
       <c r="A87" s="266" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B87" s="285" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C87" s="286" t="n">
         <v>52</v>
@@ -12956,7 +12953,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="88">
       <c r="A88" s="266"/>
       <c r="B88" s="285" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C88" s="286" t="n">
         <v>53</v>
@@ -12969,10 +12966,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="89">
       <c r="A89" s="266" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B89" s="285" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C89" s="286" t="n">
         <v>54</v>
@@ -12986,7 +12983,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="90">
       <c r="A90" s="266"/>
       <c r="B90" s="285" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C90" s="286" t="n">
         <v>55</v>
@@ -12999,7 +12996,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="91">
       <c r="A91" s="266" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B91" s="285" t="s">
         <v>41</v>
@@ -13015,7 +13012,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="92">
       <c r="A92" s="266" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B92" s="285" t="s">
         <v>42</v>
@@ -13031,10 +13028,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="93">
       <c r="A93" s="266" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B93" s="285" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C93" s="286" t="n">
         <v>58</v>
@@ -13047,7 +13044,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="94">
       <c r="A94" s="266" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B94" s="285" t="s">
         <v>75</v>
@@ -13063,10 +13060,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="95">
       <c r="A95" s="266" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B95" s="267" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C95" s="286" t="n">
         <v>60</v>
@@ -13079,10 +13076,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="96">
       <c r="A96" s="266" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B96" s="267" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C96" s="286" t="n">
         <v>61</v>
@@ -13095,10 +13092,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="97">
       <c r="A97" s="266" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B97" s="267" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C97" s="286" t="n">
         <v>62</v>
@@ -13111,10 +13108,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="98">
       <c r="A98" s="266" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B98" s="267" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C98" s="286" t="n">
         <v>63</v>
@@ -13127,10 +13124,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="99">
       <c r="A99" s="266" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B99" s="267" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C99" s="286" t="n">
         <v>64</v>
@@ -13143,10 +13140,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="100">
       <c r="A100" s="266" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B100" s="267" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C100" s="286" t="n">
         <v>65</v>
@@ -13159,10 +13156,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="101">
       <c r="A101" s="266" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B101" s="287" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C101" s="286" t="n">
         <v>66</v>
@@ -13195,10 +13192,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="104">
       <c r="A104" s="266" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B104" s="285" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C104" s="255"/>
       <c r="D104" s="131"/>
@@ -13209,10 +13206,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="105">
       <c r="A105" s="266" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B105" s="268" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C105" s="131"/>
       <c r="D105" s="131"/>
@@ -13223,10 +13220,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="106">
       <c r="A106" s="266" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B106" s="268" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C106" s="131"/>
       <c r="D106" s="131"/>
@@ -13237,10 +13234,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="107">
       <c r="A107" s="266" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B107" s="268" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C107" s="131"/>
       <c r="D107" s="131"/>
@@ -13251,10 +13248,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="108">
       <c r="A108" s="266" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B108" s="268" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C108" s="131"/>
       <c r="D108" s="131"/>
@@ -13265,10 +13262,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="109">
       <c r="A109" s="266" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B109" s="268" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C109" s="131"/>
       <c r="D109" s="131"/>
@@ -13279,7 +13276,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="110">
       <c r="A110" s="266" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B110" s="268" t="s">
         <v>76</v>
@@ -13293,7 +13290,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="111">
       <c r="A111" s="266" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B111" s="268" t="s">
         <v>77</v>
@@ -13307,7 +13304,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="112">
       <c r="A112" s="266" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B112" s="268" t="s">
         <v>78</v>
@@ -13321,7 +13318,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="113">
       <c r="A113" s="266" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B113" s="268" t="s">
         <v>34</v>
@@ -13335,7 +13332,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="114">
       <c r="A114" s="266" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B114" s="268" t="s">
         <v>35</v>
@@ -13349,7 +13346,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="115">
       <c r="A115" s="266" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B115" s="267" t="s">
         <v>36</v>
@@ -13363,7 +13360,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="116">
       <c r="A116" s="266" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B116" s="267" t="s">
         <v>37</v>
@@ -13377,15 +13374,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.25" outlineLevel="0" r="117">
       <c r="A117" s="266" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B117" s="286" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C117" s="131"/>
       <c r="D117" s="131"/>
       <c r="E117" s="242" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F117" s="131"/>
       <c r="G117" s="131"/>
@@ -13403,13 +13400,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="119">
       <c r="A119" s="292" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B119" s="293" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C119" s="294" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D119" s="131"/>
       <c r="E119" s="131"/>
@@ -13419,13 +13416,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="120">
       <c r="A120" s="295" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B120" s="295" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C120" s="296" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D120" s="131"/>
       <c r="E120" s="131"/>
@@ -13435,13 +13432,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="121">
       <c r="A121" s="295" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B121" s="295" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C121" s="297" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D121" s="131"/>
       <c r="E121" s="131"/>
@@ -13451,10 +13448,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="122">
       <c r="A122" s="298" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B122" s="295" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C122" s="299" t="n">
         <v>50</v>
@@ -13467,10 +13464,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="123">
       <c r="A123" s="298" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B123" s="295" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C123" s="297" t="n">
         <v>54</v>
@@ -13483,13 +13480,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="124">
       <c r="A124" s="298" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B124" s="295" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C124" s="297" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="D124" s="131"/>
       <c r="E124" s="131"/>
@@ -13499,13 +13496,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="125">
       <c r="A125" s="298" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B125" s="295" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C125" s="297" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D125" s="131"/>
       <c r="E125" s="131"/>
@@ -13515,10 +13512,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="126">
       <c r="A126" s="298" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B126" s="295" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C126" s="297" t="n">
         <v>33</v>
@@ -13531,10 +13528,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="127">
       <c r="A127" s="298" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B127" s="295" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C127" s="297" t="n">
         <v>35</v>
@@ -13547,10 +13544,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="128">
       <c r="A128" s="298" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B128" s="295" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C128" s="297" t="n">
         <v>37</v>
@@ -13563,10 +13560,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="129">
       <c r="A129" s="298" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B129" s="295" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C129" s="297" t="n">
         <v>42</v>
@@ -13579,10 +13576,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="130">
       <c r="A130" s="298" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B130" s="295" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C130" s="297" t="n">
         <v>46</v>
@@ -13595,10 +13592,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="131">
       <c r="A131" s="298" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B131" s="295" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C131" s="299"/>
       <c r="D131" s="131"/>
@@ -13658,8 +13655,8 @@
   </sheetPr>
   <dimension ref="A2:E3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E4" activeCellId="0" pane="topLeft" sqref="E4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="E4" activeCellId="1" pane="topLeft" sqref="R8 E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -13674,30 +13671,30 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="2">
       <c r="A2" s="301" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B2" s="302" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C2" s="303" t="n">
         <v>34</v>
       </c>
       <c r="E2" s="304" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="3">
       <c r="A3" s="301" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B3" s="305" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C3" s="306" t="n">
         <v>45</v>
       </c>
       <c r="E3" s="300" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>